<commit_message>
refatorando relatorio de pedidos diario
</commit_message>
<xml_diff>
--- a/mordomo/programas/excel/coloca_preco_custo_faltantes.xlsx
+++ b/mordomo/programas/excel/coloca_preco_custo_faltantes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\cadastro-aton\mordomo\programas\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9DE1DF3-A344-497E-8C5C-2E19AAEC4FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC56EAD-31FD-40FB-A912-60456951623C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="840" windowWidth="19440" windowHeight="15000" xr2:uid="{7E6CF1C4-1DAC-40B1-A68D-FEC71BA5C4AE}"/>
+    <workbookView xWindow="11235" yWindow="1815" windowWidth="16260" windowHeight="13905" xr2:uid="{7E6CF1C4-1DAC-40B1-A68D-FEC71BA5C4AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>Descrição</t>
   </si>
   <si>
-    <t>Vlr. Custo</t>
-  </si>
-  <si>
     <t>DG300032</t>
   </si>
   <si>
@@ -1716,6 +1713,9 @@
   </si>
   <si>
     <t xml:space="preserve">VASILHA DAGG ANTIBACTERIANA TRANSLUCIDO </t>
+  </si>
+  <si>
+    <t>CUSTO</t>
   </si>
 </sst>
 </file>
@@ -1751,8 +1751,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2069,7 +2070,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB0B5C45-A4E2-40F8-BE3E-2BD8FFCF7AB4}">
   <dimension ref="A1:D282"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2087,7 +2090,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>560</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2095,12 +2098,12 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>18.55</v>
       </c>
     </row>
@@ -2109,10 +2112,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
       </c>
       <c r="D3">
         <v>80</v>
@@ -2123,10 +2126,10 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
         <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
       </c>
       <c r="D4">
         <v>65</v>
@@ -2137,10 +2140,10 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
         <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
       </c>
       <c r="D5">
         <v>30</v>
@@ -2151,10 +2154,10 @@
         <v>1438</v>
       </c>
       <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
         <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
       </c>
       <c r="D6">
         <v>30</v>
@@ -2165,10 +2168,10 @@
         <v>1376</v>
       </c>
       <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
         <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
       </c>
       <c r="D7">
         <v>30</v>
@@ -2179,10 +2182,10 @@
         <v>696</v>
       </c>
       <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
         <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
       </c>
       <c r="D8">
         <v>40</v>
@@ -2193,10 +2196,10 @@
         <v>849</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9">
         <v>40</v>
@@ -2207,10 +2210,10 @@
         <v>25</v>
       </c>
       <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
         <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>20</v>
       </c>
       <c r="D10">
         <v>15</v>
@@ -2221,10 +2224,10 @@
         <v>620</v>
       </c>
       <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
         <v>21</v>
-      </c>
-      <c r="C11" t="s">
-        <v>22</v>
       </c>
       <c r="D11">
         <v>36.799999999999997</v>
@@ -2235,10 +2238,10 @@
         <v>27</v>
       </c>
       <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
         <v>23</v>
-      </c>
-      <c r="C12" t="s">
-        <v>24</v>
       </c>
       <c r="D12">
         <v>33.799999999999997</v>
@@ -2249,10 +2252,10 @@
         <v>709</v>
       </c>
       <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
         <v>25</v>
-      </c>
-      <c r="C13" t="s">
-        <v>26</v>
       </c>
       <c r="D13">
         <v>36.729999999999997</v>
@@ -2263,10 +2266,10 @@
         <v>38</v>
       </c>
       <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
         <v>27</v>
-      </c>
-      <c r="C14" t="s">
-        <v>28</v>
       </c>
       <c r="D14">
         <v>54.25</v>
@@ -2277,10 +2280,10 @@
         <v>42</v>
       </c>
       <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" t="s">
         <v>29</v>
-      </c>
-      <c r="C15" t="s">
-        <v>30</v>
       </c>
       <c r="D15">
         <v>80.19</v>
@@ -2291,10 +2294,10 @@
         <v>45</v>
       </c>
       <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" t="s">
         <v>31</v>
-      </c>
-      <c r="C16" t="s">
-        <v>32</v>
       </c>
       <c r="D16">
         <v>94.84</v>
@@ -2305,10 +2308,10 @@
         <v>51</v>
       </c>
       <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" t="s">
         <v>33</v>
-      </c>
-      <c r="C17" t="s">
-        <v>34</v>
       </c>
       <c r="D17">
         <v>80.42</v>
@@ -2319,10 +2322,10 @@
         <v>65</v>
       </c>
       <c r="B18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" t="s">
         <v>35</v>
-      </c>
-      <c r="C18" t="s">
-        <v>36</v>
       </c>
       <c r="D18">
         <v>54.25</v>
@@ -2333,10 +2336,10 @@
         <v>72</v>
       </c>
       <c r="B19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" t="s">
         <v>37</v>
-      </c>
-      <c r="C19" t="s">
-        <v>38</v>
       </c>
       <c r="D19">
         <v>33.47</v>
@@ -2347,10 +2350,10 @@
         <v>76</v>
       </c>
       <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" t="s">
         <v>39</v>
-      </c>
-      <c r="C20" t="s">
-        <v>40</v>
       </c>
       <c r="D20">
         <v>97.9</v>
@@ -2361,10 +2364,10 @@
         <v>1344</v>
       </c>
       <c r="B21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" t="s">
         <v>41</v>
-      </c>
-      <c r="C21" t="s">
-        <v>42</v>
       </c>
       <c r="D21">
         <v>38.44</v>
@@ -2375,10 +2378,10 @@
         <v>1337</v>
       </c>
       <c r="B22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" t="s">
         <v>43</v>
-      </c>
-      <c r="C22" t="s">
-        <v>44</v>
       </c>
       <c r="D22">
         <v>38.44</v>
@@ -2389,10 +2392,10 @@
         <v>1342</v>
       </c>
       <c r="B23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" t="s">
         <v>45</v>
-      </c>
-      <c r="C23" t="s">
-        <v>46</v>
       </c>
       <c r="D23">
         <v>28.56</v>
@@ -2403,10 +2406,10 @@
         <v>792</v>
       </c>
       <c r="B24" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" t="s">
         <v>47</v>
-      </c>
-      <c r="C24" t="s">
-        <v>48</v>
       </c>
       <c r="D24">
         <v>20.75</v>
@@ -2417,10 +2420,10 @@
         <v>844</v>
       </c>
       <c r="B25" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" t="s">
         <v>49</v>
-      </c>
-      <c r="C25" t="s">
-        <v>50</v>
       </c>
       <c r="D25">
         <v>12.63</v>
@@ -2431,10 +2434,10 @@
         <v>129</v>
       </c>
       <c r="B26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" t="s">
         <v>51</v>
-      </c>
-      <c r="C26" t="s">
-        <v>52</v>
       </c>
       <c r="D26">
         <v>18.5</v>
@@ -2445,10 +2448,10 @@
         <v>107</v>
       </c>
       <c r="B27" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" t="s">
         <v>53</v>
-      </c>
-      <c r="C27" t="s">
-        <v>54</v>
       </c>
       <c r="D27">
         <v>90</v>
@@ -2459,10 +2462,10 @@
         <v>137</v>
       </c>
       <c r="B28" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" t="s">
         <v>55</v>
-      </c>
-      <c r="C28" t="s">
-        <v>56</v>
       </c>
       <c r="D28">
         <v>25</v>
@@ -2473,10 +2476,10 @@
         <v>124</v>
       </c>
       <c r="B29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" t="s">
         <v>57</v>
-      </c>
-      <c r="C29" t="s">
-        <v>58</v>
       </c>
       <c r="D29">
         <v>50</v>
@@ -2487,10 +2490,10 @@
         <v>125</v>
       </c>
       <c r="B30" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" t="s">
         <v>59</v>
-      </c>
-      <c r="C30" t="s">
-        <v>60</v>
       </c>
       <c r="D30">
         <v>50</v>
@@ -2501,10 +2504,10 @@
         <v>128</v>
       </c>
       <c r="B31" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" t="s">
         <v>61</v>
-      </c>
-      <c r="C31" t="s">
-        <v>62</v>
       </c>
       <c r="D31">
         <v>50</v>
@@ -2515,10 +2518,10 @@
         <v>119</v>
       </c>
       <c r="B32" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" t="s">
         <v>63</v>
-      </c>
-      <c r="C32" t="s">
-        <v>64</v>
       </c>
       <c r="D32">
         <v>60</v>
@@ -2529,10 +2532,10 @@
         <v>104</v>
       </c>
       <c r="B33" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" t="s">
         <v>65</v>
-      </c>
-      <c r="C33" t="s">
-        <v>66</v>
       </c>
       <c r="D33">
         <v>60</v>
@@ -2543,10 +2546,10 @@
         <v>112</v>
       </c>
       <c r="B34" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" t="s">
         <v>67</v>
-      </c>
-      <c r="C34" t="s">
-        <v>68</v>
       </c>
       <c r="D34">
         <v>62.79</v>
@@ -2557,10 +2560,10 @@
         <v>132</v>
       </c>
       <c r="B35" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" t="s">
         <v>69</v>
-      </c>
-      <c r="C35" t="s">
-        <v>70</v>
       </c>
       <c r="D35">
         <v>25</v>
@@ -2571,10 +2574,10 @@
         <v>1431</v>
       </c>
       <c r="B36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36" t="s">
         <v>71</v>
-      </c>
-      <c r="C36" t="s">
-        <v>72</v>
       </c>
       <c r="D36">
         <v>20.190000000000001</v>
@@ -2585,10 +2588,10 @@
         <v>1427</v>
       </c>
       <c r="B37" t="s">
+        <v>72</v>
+      </c>
+      <c r="C37" t="s">
         <v>73</v>
-      </c>
-      <c r="C37" t="s">
-        <v>74</v>
       </c>
       <c r="D37">
         <v>35.79</v>
@@ -2599,10 +2602,10 @@
         <v>617</v>
       </c>
       <c r="B38" t="s">
+        <v>74</v>
+      </c>
+      <c r="C38" t="s">
         <v>75</v>
-      </c>
-      <c r="C38" t="s">
-        <v>76</v>
       </c>
       <c r="D38">
         <v>23.9</v>
@@ -2613,10 +2616,10 @@
         <v>615</v>
       </c>
       <c r="B39" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39" t="s">
         <v>77</v>
-      </c>
-      <c r="C39" t="s">
-        <v>78</v>
       </c>
       <c r="D39">
         <v>23.9</v>
@@ -2627,10 +2630,10 @@
         <v>1260</v>
       </c>
       <c r="B40" t="s">
+        <v>78</v>
+      </c>
+      <c r="C40" t="s">
         <v>79</v>
-      </c>
-      <c r="C40" t="s">
-        <v>80</v>
       </c>
       <c r="D40">
         <v>43.65</v>
@@ -2641,10 +2644,10 @@
         <v>1255</v>
       </c>
       <c r="B41" t="s">
+        <v>80</v>
+      </c>
+      <c r="C41" t="s">
         <v>81</v>
-      </c>
-      <c r="C41" t="s">
-        <v>82</v>
       </c>
       <c r="D41">
         <v>43.65</v>
@@ -2655,10 +2658,10 @@
         <v>1250</v>
       </c>
       <c r="B42" t="s">
+        <v>82</v>
+      </c>
+      <c r="C42" t="s">
         <v>83</v>
-      </c>
-      <c r="C42" t="s">
-        <v>84</v>
       </c>
       <c r="D42">
         <v>43.65</v>
@@ -2669,10 +2672,10 @@
         <v>81</v>
       </c>
       <c r="B43" t="s">
+        <v>84</v>
+      </c>
+      <c r="C43" t="s">
         <v>85</v>
-      </c>
-      <c r="C43" t="s">
-        <v>86</v>
       </c>
       <c r="D43">
         <v>29.8</v>
@@ -2683,10 +2686,10 @@
         <v>610</v>
       </c>
       <c r="B44" t="s">
+        <v>86</v>
+      </c>
+      <c r="C44" t="s">
         <v>87</v>
-      </c>
-      <c r="C44" t="s">
-        <v>88</v>
       </c>
       <c r="D44">
         <v>29.8</v>
@@ -2697,10 +2700,10 @@
         <v>1278</v>
       </c>
       <c r="B45" t="s">
+        <v>88</v>
+      </c>
+      <c r="C45" t="s">
         <v>89</v>
-      </c>
-      <c r="C45" t="s">
-        <v>90</v>
       </c>
       <c r="D45">
         <v>29.12</v>
@@ -2711,10 +2714,10 @@
         <v>1506</v>
       </c>
       <c r="B46" t="s">
+        <v>90</v>
+      </c>
+      <c r="C46" t="s">
         <v>91</v>
-      </c>
-      <c r="C46" t="s">
-        <v>92</v>
       </c>
       <c r="D46">
         <v>8.82</v>
@@ -2725,10 +2728,10 @@
         <v>1501</v>
       </c>
       <c r="B47" t="s">
+        <v>92</v>
+      </c>
+      <c r="C47" t="s">
         <v>93</v>
-      </c>
-      <c r="C47" t="s">
-        <v>94</v>
       </c>
       <c r="D47">
         <v>8.82</v>
@@ -2739,10 +2742,10 @@
         <v>1439</v>
       </c>
       <c r="B48" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" t="s">
         <v>95</v>
-      </c>
-      <c r="C48" t="s">
-        <v>96</v>
       </c>
       <c r="D48">
         <v>35.479999999999997</v>
@@ -2753,10 +2756,10 @@
         <v>746</v>
       </c>
       <c r="B49" t="s">
+        <v>96</v>
+      </c>
+      <c r="C49" t="s">
         <v>97</v>
-      </c>
-      <c r="C49" t="s">
-        <v>98</v>
       </c>
       <c r="D49">
         <v>36.119999999999997</v>
@@ -2767,10 +2770,10 @@
         <v>747</v>
       </c>
       <c r="B50" t="s">
+        <v>98</v>
+      </c>
+      <c r="C50" t="s">
         <v>99</v>
-      </c>
-      <c r="C50" t="s">
-        <v>100</v>
       </c>
       <c r="D50">
         <v>40.25</v>
@@ -2781,10 +2784,10 @@
         <v>749</v>
       </c>
       <c r="B51" t="s">
+        <v>100</v>
+      </c>
+      <c r="C51" t="s">
         <v>101</v>
-      </c>
-      <c r="C51" t="s">
-        <v>102</v>
       </c>
       <c r="D51">
         <v>49.62</v>
@@ -2795,10 +2798,10 @@
         <v>743</v>
       </c>
       <c r="B52" t="s">
+        <v>102</v>
+      </c>
+      <c r="C52" t="s">
         <v>103</v>
-      </c>
-      <c r="C52" t="s">
-        <v>104</v>
       </c>
       <c r="D52">
         <v>50</v>
@@ -2809,10 +2812,10 @@
         <v>793</v>
       </c>
       <c r="B53" t="s">
+        <v>104</v>
+      </c>
+      <c r="C53" t="s">
         <v>105</v>
-      </c>
-      <c r="C53" t="s">
-        <v>106</v>
       </c>
       <c r="D53">
         <v>34.29</v>
@@ -2823,10 +2826,10 @@
         <v>794</v>
       </c>
       <c r="B54" t="s">
+        <v>106</v>
+      </c>
+      <c r="C54" t="s">
         <v>107</v>
-      </c>
-      <c r="C54" t="s">
-        <v>108</v>
       </c>
       <c r="D54">
         <v>34.29</v>
@@ -2837,10 +2840,10 @@
         <v>795</v>
       </c>
       <c r="B55" t="s">
+        <v>108</v>
+      </c>
+      <c r="C55" t="s">
         <v>109</v>
-      </c>
-      <c r="C55" t="s">
-        <v>110</v>
       </c>
       <c r="D55">
         <v>34.29</v>
@@ -2851,10 +2854,10 @@
         <v>840</v>
       </c>
       <c r="B56" t="s">
+        <v>110</v>
+      </c>
+      <c r="C56" t="s">
         <v>111</v>
-      </c>
-      <c r="C56" t="s">
-        <v>112</v>
       </c>
       <c r="D56">
         <v>60.42</v>
@@ -2865,10 +2868,10 @@
         <v>841</v>
       </c>
       <c r="B57" t="s">
+        <v>112</v>
+      </c>
+      <c r="C57" t="s">
         <v>113</v>
-      </c>
-      <c r="C57" t="s">
-        <v>114</v>
       </c>
       <c r="D57">
         <v>60.53</v>
@@ -2879,10 +2882,10 @@
         <v>1521</v>
       </c>
       <c r="B58" t="s">
+        <v>114</v>
+      </c>
+      <c r="C58" t="s">
         <v>115</v>
-      </c>
-      <c r="C58" t="s">
-        <v>116</v>
       </c>
       <c r="D58">
         <v>53.65</v>
@@ -2893,10 +2896,10 @@
         <v>1524</v>
       </c>
       <c r="B59" t="s">
+        <v>116</v>
+      </c>
+      <c r="C59" t="s">
         <v>117</v>
-      </c>
-      <c r="C59" t="s">
-        <v>118</v>
       </c>
       <c r="D59">
         <v>53.65</v>
@@ -2907,10 +2910,10 @@
         <v>1523</v>
       </c>
       <c r="B60" t="s">
+        <v>118</v>
+      </c>
+      <c r="C60" t="s">
         <v>119</v>
-      </c>
-      <c r="C60" t="s">
-        <v>120</v>
       </c>
       <c r="D60">
         <v>53.65</v>
@@ -2921,10 +2924,10 @@
         <v>1522</v>
       </c>
       <c r="B61" t="s">
+        <v>120</v>
+      </c>
+      <c r="C61" t="s">
         <v>121</v>
-      </c>
-      <c r="C61" t="s">
-        <v>122</v>
       </c>
       <c r="D61">
         <v>53.65</v>
@@ -2935,10 +2938,10 @@
         <v>814</v>
       </c>
       <c r="B62" t="s">
+        <v>122</v>
+      </c>
+      <c r="C62" t="s">
         <v>123</v>
-      </c>
-      <c r="C62" t="s">
-        <v>124</v>
       </c>
       <c r="D62">
         <v>20</v>
@@ -2949,10 +2952,10 @@
         <v>101</v>
       </c>
       <c r="B63" t="s">
+        <v>124</v>
+      </c>
+      <c r="C63" t="s">
         <v>125</v>
-      </c>
-      <c r="C63" t="s">
-        <v>126</v>
       </c>
       <c r="D63">
         <v>40</v>
@@ -2963,10 +2966,10 @@
         <v>98</v>
       </c>
       <c r="B64" t="s">
+        <v>126</v>
+      </c>
+      <c r="C64" t="s">
         <v>127</v>
-      </c>
-      <c r="C64" t="s">
-        <v>128</v>
       </c>
       <c r="D64">
         <v>60</v>
@@ -2977,10 +2980,10 @@
         <v>100</v>
       </c>
       <c r="B65" t="s">
+        <v>128</v>
+      </c>
+      <c r="C65" t="s">
         <v>129</v>
-      </c>
-      <c r="C65" t="s">
-        <v>130</v>
       </c>
       <c r="D65">
         <v>60</v>
@@ -2991,10 +2994,10 @@
         <v>79</v>
       </c>
       <c r="B66" t="s">
+        <v>130</v>
+      </c>
+      <c r="C66" t="s">
         <v>131</v>
-      </c>
-      <c r="C66" t="s">
-        <v>132</v>
       </c>
       <c r="D66">
         <v>1.57</v>
@@ -3005,10 +3008,10 @@
         <v>1495</v>
       </c>
       <c r="B67" t="s">
+        <v>132</v>
+      </c>
+      <c r="C67" t="s">
         <v>133</v>
-      </c>
-      <c r="C67" t="s">
-        <v>134</v>
       </c>
       <c r="D67">
         <v>21.25</v>
@@ -3019,10 +3022,10 @@
         <v>1055</v>
       </c>
       <c r="B68" t="s">
+        <v>134</v>
+      </c>
+      <c r="C68" t="s">
         <v>135</v>
-      </c>
-      <c r="C68" t="s">
-        <v>136</v>
       </c>
       <c r="D68">
         <v>21.25</v>
@@ -3033,10 +3036,10 @@
         <v>1071</v>
       </c>
       <c r="B69" t="s">
+        <v>136</v>
+      </c>
+      <c r="C69" t="s">
         <v>137</v>
-      </c>
-      <c r="C69" t="s">
-        <v>138</v>
       </c>
       <c r="D69">
         <v>21.25</v>
@@ -3047,10 +3050,10 @@
         <v>1072</v>
       </c>
       <c r="B70" t="s">
+        <v>138</v>
+      </c>
+      <c r="C70" t="s">
         <v>139</v>
-      </c>
-      <c r="C70" t="s">
-        <v>140</v>
       </c>
       <c r="D70">
         <v>21.25</v>
@@ -3061,10 +3064,10 @@
         <v>1212</v>
       </c>
       <c r="B71" t="s">
+        <v>140</v>
+      </c>
+      <c r="C71" t="s">
         <v>141</v>
-      </c>
-      <c r="C71" t="s">
-        <v>142</v>
       </c>
       <c r="D71">
         <v>21.25</v>
@@ -3075,10 +3078,10 @@
         <v>653</v>
       </c>
       <c r="B72" t="s">
+        <v>142</v>
+      </c>
+      <c r="C72" t="s">
         <v>143</v>
-      </c>
-      <c r="C72" t="s">
-        <v>144</v>
       </c>
       <c r="D72">
         <v>21.87</v>
@@ -3089,10 +3092,10 @@
         <v>658</v>
       </c>
       <c r="B73" t="s">
+        <v>144</v>
+      </c>
+      <c r="C73" t="s">
         <v>145</v>
-      </c>
-      <c r="C73" t="s">
-        <v>146</v>
       </c>
       <c r="D73">
         <v>21.87</v>
@@ -3103,10 +3106,10 @@
         <v>648</v>
       </c>
       <c r="B74" t="s">
+        <v>146</v>
+      </c>
+      <c r="C74" t="s">
         <v>147</v>
-      </c>
-      <c r="C74" t="s">
-        <v>148</v>
       </c>
       <c r="D74">
         <v>21.87</v>
@@ -3117,10 +3120,10 @@
         <v>643</v>
       </c>
       <c r="B75" t="s">
+        <v>148</v>
+      </c>
+      <c r="C75" t="s">
         <v>149</v>
-      </c>
-      <c r="C75" t="s">
-        <v>150</v>
       </c>
       <c r="D75">
         <v>22.53</v>
@@ -3131,10 +3134,10 @@
         <v>633</v>
       </c>
       <c r="B76" t="s">
+        <v>150</v>
+      </c>
+      <c r="C76" t="s">
         <v>151</v>
-      </c>
-      <c r="C76" t="s">
-        <v>152</v>
       </c>
       <c r="D76">
         <v>22.53</v>
@@ -3145,10 +3148,10 @@
         <v>628</v>
       </c>
       <c r="B77" t="s">
+        <v>152</v>
+      </c>
+      <c r="C77" t="s">
         <v>153</v>
-      </c>
-      <c r="C77" t="s">
-        <v>154</v>
       </c>
       <c r="D77">
         <v>22.53</v>
@@ -3159,10 +3162,10 @@
         <v>638</v>
       </c>
       <c r="B78" t="s">
+        <v>154</v>
+      </c>
+      <c r="C78" t="s">
         <v>155</v>
-      </c>
-      <c r="C78" t="s">
-        <v>156</v>
       </c>
       <c r="D78">
         <v>22.53</v>
@@ -3173,10 +3176,10 @@
         <v>1028</v>
       </c>
       <c r="B79" t="s">
+        <v>156</v>
+      </c>
+      <c r="C79" t="s">
         <v>157</v>
-      </c>
-      <c r="C79" t="s">
-        <v>158</v>
       </c>
       <c r="D79">
         <v>21.25</v>
@@ -3187,10 +3190,10 @@
         <v>1042</v>
       </c>
       <c r="B80" t="s">
+        <v>158</v>
+      </c>
+      <c r="C80" t="s">
         <v>159</v>
-      </c>
-      <c r="C80" t="s">
-        <v>160</v>
       </c>
       <c r="D80">
         <v>21.25</v>
@@ -3201,10 +3204,10 @@
         <v>1037</v>
       </c>
       <c r="B81" t="s">
+        <v>160</v>
+      </c>
+      <c r="C81" t="s">
         <v>161</v>
-      </c>
-      <c r="C81" t="s">
-        <v>162</v>
       </c>
       <c r="D81">
         <v>21.25</v>
@@ -3215,10 +3218,10 @@
         <v>1046</v>
       </c>
       <c r="B82" t="s">
+        <v>162</v>
+      </c>
+      <c r="C82" t="s">
         <v>163</v>
-      </c>
-      <c r="C82" t="s">
-        <v>164</v>
       </c>
       <c r="D82">
         <v>21.25</v>
@@ -3229,10 +3232,10 @@
         <v>1041</v>
       </c>
       <c r="B83" t="s">
+        <v>164</v>
+      </c>
+      <c r="C83" t="s">
         <v>165</v>
-      </c>
-      <c r="C83" t="s">
-        <v>166</v>
       </c>
       <c r="D83">
         <v>21.25</v>
@@ -3243,10 +3246,10 @@
         <v>1047</v>
       </c>
       <c r="B84" t="s">
+        <v>166</v>
+      </c>
+      <c r="C84" t="s">
         <v>167</v>
-      </c>
-      <c r="C84" t="s">
-        <v>168</v>
       </c>
       <c r="D84">
         <v>21.25</v>
@@ -3257,10 +3260,10 @@
         <v>1027</v>
       </c>
       <c r="B85" t="s">
+        <v>168</v>
+      </c>
+      <c r="C85" t="s">
         <v>169</v>
-      </c>
-      <c r="C85" t="s">
-        <v>170</v>
       </c>
       <c r="D85">
         <v>21.25</v>
@@ -3271,10 +3274,10 @@
         <v>1054</v>
       </c>
       <c r="B86" t="s">
+        <v>170</v>
+      </c>
+      <c r="C86" t="s">
         <v>171</v>
-      </c>
-      <c r="C86" t="s">
-        <v>172</v>
       </c>
       <c r="D86">
         <v>31.52</v>
@@ -3285,10 +3288,10 @@
         <v>1298</v>
       </c>
       <c r="B87" t="s">
+        <v>172</v>
+      </c>
+      <c r="C87" t="s">
         <v>173</v>
-      </c>
-      <c r="C87" t="s">
-        <v>174</v>
       </c>
       <c r="D87">
         <v>32.4</v>
@@ -3299,10 +3302,10 @@
         <v>1182</v>
       </c>
       <c r="B88" t="s">
+        <v>174</v>
+      </c>
+      <c r="C88" t="s">
         <v>175</v>
-      </c>
-      <c r="C88" t="s">
-        <v>176</v>
       </c>
       <c r="D88">
         <v>35.130000000000003</v>
@@ -3313,10 +3316,10 @@
         <v>1308</v>
       </c>
       <c r="B89" t="s">
+        <v>176</v>
+      </c>
+      <c r="C89" t="s">
         <v>177</v>
-      </c>
-      <c r="C89" t="s">
-        <v>178</v>
       </c>
       <c r="D89">
         <v>32.4</v>
@@ -3327,10 +3330,10 @@
         <v>1241</v>
       </c>
       <c r="B90" t="s">
+        <v>178</v>
+      </c>
+      <c r="C90" t="s">
         <v>179</v>
-      </c>
-      <c r="C90" t="s">
-        <v>180</v>
       </c>
       <c r="D90">
         <v>23.3</v>
@@ -3341,10 +3344,10 @@
         <v>852</v>
       </c>
       <c r="B91" t="s">
+        <v>180</v>
+      </c>
+      <c r="C91" t="s">
         <v>181</v>
-      </c>
-      <c r="C91" t="s">
-        <v>182</v>
       </c>
       <c r="D91">
         <v>44.22</v>
@@ -3355,10 +3358,10 @@
         <v>853</v>
       </c>
       <c r="B92" t="s">
+        <v>182</v>
+      </c>
+      <c r="C92" t="s">
         <v>183</v>
-      </c>
-      <c r="C92" t="s">
-        <v>184</v>
       </c>
       <c r="D92">
         <v>79.63</v>
@@ -3369,10 +3372,10 @@
         <v>1289</v>
       </c>
       <c r="B93" t="s">
+        <v>184</v>
+      </c>
+      <c r="C93" t="s">
         <v>185</v>
-      </c>
-      <c r="C93" t="s">
-        <v>186</v>
       </c>
       <c r="D93">
         <v>12</v>
@@ -3383,10 +3386,10 @@
         <v>1334</v>
       </c>
       <c r="B94" t="s">
+        <v>186</v>
+      </c>
+      <c r="C94" t="s">
         <v>187</v>
-      </c>
-      <c r="C94" t="s">
-        <v>188</v>
       </c>
       <c r="D94">
         <v>12</v>
@@ -3397,10 +3400,10 @@
         <v>1333</v>
       </c>
       <c r="B95" t="s">
+        <v>188</v>
+      </c>
+      <c r="C95" t="s">
         <v>189</v>
-      </c>
-      <c r="C95" t="s">
-        <v>190</v>
       </c>
       <c r="D95">
         <v>12</v>
@@ -3411,10 +3414,10 @@
         <v>1335</v>
       </c>
       <c r="B96" t="s">
+        <v>190</v>
+      </c>
+      <c r="C96" t="s">
         <v>191</v>
-      </c>
-      <c r="C96" t="s">
-        <v>192</v>
       </c>
       <c r="D96">
         <v>12</v>
@@ -3425,10 +3428,10 @@
         <v>153</v>
       </c>
       <c r="B97" t="s">
+        <v>192</v>
+      </c>
+      <c r="C97" t="s">
         <v>193</v>
-      </c>
-      <c r="C97" t="s">
-        <v>194</v>
       </c>
       <c r="D97">
         <v>37</v>
@@ -3439,10 +3442,10 @@
         <v>158</v>
       </c>
       <c r="B98" t="s">
+        <v>194</v>
+      </c>
+      <c r="C98" t="s">
         <v>195</v>
-      </c>
-      <c r="C98" t="s">
-        <v>196</v>
       </c>
       <c r="D98">
         <v>50</v>
@@ -3453,10 +3456,10 @@
         <v>159</v>
       </c>
       <c r="B99" t="s">
+        <v>196</v>
+      </c>
+      <c r="C99" t="s">
         <v>197</v>
-      </c>
-      <c r="C99" t="s">
-        <v>198</v>
       </c>
       <c r="D99">
         <v>12.14</v>
@@ -3467,10 +3470,10 @@
         <v>681</v>
       </c>
       <c r="B100" t="s">
+        <v>198</v>
+      </c>
+      <c r="C100" t="s">
         <v>199</v>
-      </c>
-      <c r="C100" t="s">
-        <v>200</v>
       </c>
       <c r="D100">
         <v>33.6</v>
@@ -3481,10 +3484,10 @@
         <v>789</v>
       </c>
       <c r="B101" t="s">
+        <v>200</v>
+      </c>
+      <c r="C101" t="s">
         <v>201</v>
-      </c>
-      <c r="C101" t="s">
-        <v>202</v>
       </c>
       <c r="D101">
         <v>31.53</v>
@@ -3495,10 +3498,10 @@
         <v>1511</v>
       </c>
       <c r="B102" t="s">
+        <v>202</v>
+      </c>
+      <c r="C102" t="s">
         <v>203</v>
-      </c>
-      <c r="C102" t="s">
-        <v>204</v>
       </c>
       <c r="D102">
         <v>53.1</v>
@@ -3509,10 +3512,10 @@
         <v>1009</v>
       </c>
       <c r="B103" t="s">
+        <v>204</v>
+      </c>
+      <c r="C103" t="s">
         <v>205</v>
-      </c>
-      <c r="C103" t="s">
-        <v>206</v>
       </c>
       <c r="D103">
         <v>46.08</v>
@@ -3523,10 +3526,10 @@
         <v>1518</v>
       </c>
       <c r="B104" t="s">
+        <v>206</v>
+      </c>
+      <c r="C104" t="s">
         <v>207</v>
-      </c>
-      <c r="C104" t="s">
-        <v>208</v>
       </c>
       <c r="D104">
         <v>44.73</v>
@@ -3537,10 +3540,10 @@
         <v>175</v>
       </c>
       <c r="B105" t="s">
+        <v>208</v>
+      </c>
+      <c r="C105" t="s">
         <v>209</v>
-      </c>
-      <c r="C105" t="s">
-        <v>210</v>
       </c>
       <c r="D105">
         <v>40</v>
@@ -3551,10 +3554,10 @@
         <v>176</v>
       </c>
       <c r="B106" t="s">
+        <v>210</v>
+      </c>
+      <c r="C106" t="s">
         <v>211</v>
-      </c>
-      <c r="C106" t="s">
-        <v>212</v>
       </c>
       <c r="D106">
         <v>40</v>
@@ -3565,10 +3568,10 @@
         <v>177</v>
       </c>
       <c r="B107" t="s">
+        <v>212</v>
+      </c>
+      <c r="C107" t="s">
         <v>213</v>
-      </c>
-      <c r="C107" t="s">
-        <v>214</v>
       </c>
       <c r="D107">
         <v>40</v>
@@ -3579,10 +3582,10 @@
         <v>187</v>
       </c>
       <c r="B108" t="s">
+        <v>214</v>
+      </c>
+      <c r="C108" t="s">
         <v>215</v>
-      </c>
-      <c r="C108" t="s">
-        <v>216</v>
       </c>
       <c r="D108">
         <v>30</v>
@@ -3593,10 +3596,10 @@
         <v>178</v>
       </c>
       <c r="B109" t="s">
+        <v>216</v>
+      </c>
+      <c r="C109" t="s">
         <v>217</v>
-      </c>
-      <c r="C109" t="s">
-        <v>218</v>
       </c>
       <c r="D109">
         <v>30</v>
@@ -3607,10 +3610,10 @@
         <v>169</v>
       </c>
       <c r="B110" t="s">
+        <v>218</v>
+      </c>
+      <c r="C110" t="s">
         <v>219</v>
-      </c>
-      <c r="C110" t="s">
-        <v>220</v>
       </c>
       <c r="D110">
         <v>39.9</v>
@@ -3621,10 +3624,10 @@
         <v>171</v>
       </c>
       <c r="B111" t="s">
+        <v>220</v>
+      </c>
+      <c r="C111" t="s">
         <v>221</v>
-      </c>
-      <c r="C111" t="s">
-        <v>222</v>
       </c>
       <c r="D111">
         <v>39.9</v>
@@ -3635,10 +3638,10 @@
         <v>1403</v>
       </c>
       <c r="B112" t="s">
+        <v>222</v>
+      </c>
+      <c r="C112" t="s">
         <v>223</v>
-      </c>
-      <c r="C112" t="s">
-        <v>224</v>
       </c>
       <c r="D112">
         <v>30</v>
@@ -3649,10 +3652,10 @@
         <v>163</v>
       </c>
       <c r="B113" t="s">
+        <v>224</v>
+      </c>
+      <c r="C113" t="s">
         <v>225</v>
-      </c>
-      <c r="C113" t="s">
-        <v>226</v>
       </c>
       <c r="D113">
         <v>30</v>
@@ -3663,10 +3666,10 @@
         <v>164</v>
       </c>
       <c r="B114" t="s">
+        <v>226</v>
+      </c>
+      <c r="C114" t="s">
         <v>227</v>
-      </c>
-      <c r="C114" t="s">
-        <v>228</v>
       </c>
       <c r="D114">
         <v>30</v>
@@ -3677,10 +3680,10 @@
         <v>166</v>
       </c>
       <c r="B115" t="s">
+        <v>228</v>
+      </c>
+      <c r="C115" t="s">
         <v>229</v>
-      </c>
-      <c r="C115" t="s">
-        <v>230</v>
       </c>
       <c r="D115">
         <v>30</v>
@@ -3691,10 +3694,10 @@
         <v>1324</v>
       </c>
       <c r="B116" t="s">
+        <v>230</v>
+      </c>
+      <c r="C116" t="s">
         <v>231</v>
-      </c>
-      <c r="C116" t="s">
-        <v>232</v>
       </c>
       <c r="D116">
         <v>40</v>
@@ -3705,10 +3708,10 @@
         <v>1326</v>
       </c>
       <c r="B117" t="s">
+        <v>232</v>
+      </c>
+      <c r="C117" t="s">
         <v>233</v>
-      </c>
-      <c r="C117" t="s">
-        <v>234</v>
       </c>
       <c r="D117">
         <v>40</v>
@@ -3719,10 +3722,10 @@
         <v>1325</v>
       </c>
       <c r="B118" t="s">
+        <v>234</v>
+      </c>
+      <c r="C118" t="s">
         <v>235</v>
-      </c>
-      <c r="C118" t="s">
-        <v>236</v>
       </c>
       <c r="D118">
         <v>40</v>
@@ -3733,10 +3736,10 @@
         <v>1327</v>
       </c>
       <c r="B119" t="s">
+        <v>236</v>
+      </c>
+      <c r="C119" t="s">
         <v>237</v>
-      </c>
-      <c r="C119" t="s">
-        <v>238</v>
       </c>
       <c r="D119">
         <v>40</v>
@@ -3747,10 +3750,10 @@
         <v>1328</v>
       </c>
       <c r="B120" t="s">
+        <v>238</v>
+      </c>
+      <c r="C120" t="s">
         <v>239</v>
-      </c>
-      <c r="C120" t="s">
-        <v>240</v>
       </c>
       <c r="D120">
         <v>40</v>
@@ -3761,10 +3764,10 @@
         <v>179</v>
       </c>
       <c r="B121" t="s">
+        <v>240</v>
+      </c>
+      <c r="C121" t="s">
         <v>241</v>
-      </c>
-      <c r="C121" t="s">
-        <v>242</v>
       </c>
       <c r="D121">
         <v>44.09</v>
@@ -3775,10 +3778,10 @@
         <v>180</v>
       </c>
       <c r="B122" t="s">
+        <v>242</v>
+      </c>
+      <c r="C122" t="s">
         <v>243</v>
-      </c>
-      <c r="C122" t="s">
-        <v>244</v>
       </c>
       <c r="D122">
         <v>44.09</v>
@@ -3789,10 +3792,10 @@
         <v>182</v>
       </c>
       <c r="B123" t="s">
+        <v>244</v>
+      </c>
+      <c r="C123" t="s">
         <v>245</v>
-      </c>
-      <c r="C123" t="s">
-        <v>246</v>
       </c>
       <c r="D123">
         <v>44.09</v>
@@ -3803,10 +3806,10 @@
         <v>183</v>
       </c>
       <c r="B124" t="s">
+        <v>246</v>
+      </c>
+      <c r="C124" t="s">
         <v>247</v>
-      </c>
-      <c r="C124" t="s">
-        <v>248</v>
       </c>
       <c r="D124">
         <v>44.09</v>
@@ -3817,10 +3820,10 @@
         <v>857</v>
       </c>
       <c r="B125" t="s">
+        <v>248</v>
+      </c>
+      <c r="C125" t="s">
         <v>249</v>
-      </c>
-      <c r="C125" t="s">
-        <v>250</v>
       </c>
       <c r="D125">
         <v>23.26</v>
@@ -3831,10 +3834,10 @@
         <v>755</v>
       </c>
       <c r="B126" t="s">
+        <v>250</v>
+      </c>
+      <c r="C126" t="s">
         <v>251</v>
-      </c>
-      <c r="C126" t="s">
-        <v>252</v>
       </c>
       <c r="D126">
         <v>23.26</v>
@@ -3845,10 +3848,10 @@
         <v>194</v>
       </c>
       <c r="B127" t="s">
+        <v>252</v>
+      </c>
+      <c r="C127" t="s">
         <v>253</v>
-      </c>
-      <c r="C127" t="s">
-        <v>254</v>
       </c>
       <c r="D127">
         <v>30</v>
@@ -3859,10 +3862,10 @@
         <v>195</v>
       </c>
       <c r="B128" t="s">
+        <v>254</v>
+      </c>
+      <c r="C128" t="s">
         <v>255</v>
-      </c>
-      <c r="C128" t="s">
-        <v>256</v>
       </c>
       <c r="D128">
         <v>30</v>
@@ -3873,10 +3876,10 @@
         <v>196</v>
       </c>
       <c r="B129" t="s">
+        <v>256</v>
+      </c>
+      <c r="C129" t="s">
         <v>257</v>
-      </c>
-      <c r="C129" t="s">
-        <v>258</v>
       </c>
       <c r="D129">
         <v>30</v>
@@ -3887,10 +3890,10 @@
         <v>233</v>
       </c>
       <c r="B130" t="s">
+        <v>258</v>
+      </c>
+      <c r="C130" t="s">
         <v>259</v>
-      </c>
-      <c r="C130" t="s">
-        <v>260</v>
       </c>
       <c r="D130">
         <v>20</v>
@@ -3901,10 +3904,10 @@
         <v>234</v>
       </c>
       <c r="B131" t="s">
+        <v>260</v>
+      </c>
+      <c r="C131" t="s">
         <v>261</v>
-      </c>
-      <c r="C131" t="s">
-        <v>262</v>
       </c>
       <c r="D131">
         <v>20</v>
@@ -3915,10 +3918,10 @@
         <v>235</v>
       </c>
       <c r="B132" t="s">
+        <v>262</v>
+      </c>
+      <c r="C132" t="s">
         <v>263</v>
-      </c>
-      <c r="C132" t="s">
-        <v>264</v>
       </c>
       <c r="D132">
         <v>20</v>
@@ -3929,10 +3932,10 @@
         <v>225</v>
       </c>
       <c r="B133" t="s">
+        <v>264</v>
+      </c>
+      <c r="C133" t="s">
         <v>265</v>
-      </c>
-      <c r="C133" t="s">
-        <v>266</v>
       </c>
       <c r="D133">
         <v>42.76</v>
@@ -3943,10 +3946,10 @@
         <v>189</v>
       </c>
       <c r="B134" t="s">
+        <v>266</v>
+      </c>
+      <c r="C134" t="s">
         <v>267</v>
-      </c>
-      <c r="C134" t="s">
-        <v>268</v>
       </c>
       <c r="D134">
         <v>21.2</v>
@@ -3957,10 +3960,10 @@
         <v>190</v>
       </c>
       <c r="B135" t="s">
+        <v>268</v>
+      </c>
+      <c r="C135" t="s">
         <v>269</v>
-      </c>
-      <c r="C135" t="s">
-        <v>270</v>
       </c>
       <c r="D135">
         <v>21.2</v>
@@ -3971,10 +3974,10 @@
         <v>236</v>
       </c>
       <c r="B136" t="s">
+        <v>270</v>
+      </c>
+      <c r="C136" t="s">
         <v>271</v>
-      </c>
-      <c r="C136" t="s">
-        <v>272</v>
       </c>
       <c r="D136">
         <v>47.27</v>
@@ -3985,10 +3988,10 @@
         <v>198</v>
       </c>
       <c r="B137" t="s">
+        <v>272</v>
+      </c>
+      <c r="C137" t="s">
         <v>273</v>
-      </c>
-      <c r="C137" t="s">
-        <v>274</v>
       </c>
       <c r="D137">
         <v>28.29</v>
@@ -3999,10 +4002,10 @@
         <v>1517</v>
       </c>
       <c r="B138" t="s">
+        <v>274</v>
+      </c>
+      <c r="C138" t="s">
         <v>275</v>
-      </c>
-      <c r="C138" t="s">
-        <v>276</v>
       </c>
       <c r="D138">
         <v>28.29</v>
@@ -4013,10 +4016,10 @@
         <v>334</v>
       </c>
       <c r="B139" t="s">
+        <v>276</v>
+      </c>
+      <c r="C139" t="s">
         <v>277</v>
-      </c>
-      <c r="C139" t="s">
-        <v>278</v>
       </c>
       <c r="D139">
         <v>50</v>
@@ -4027,10 +4030,10 @@
         <v>339</v>
       </c>
       <c r="B140" t="s">
+        <v>278</v>
+      </c>
+      <c r="C140" t="s">
         <v>279</v>
-      </c>
-      <c r="C140" t="s">
-        <v>280</v>
       </c>
       <c r="D140">
         <v>50</v>
@@ -4041,10 +4044,10 @@
         <v>343</v>
       </c>
       <c r="B141" t="s">
+        <v>280</v>
+      </c>
+      <c r="C141" t="s">
         <v>281</v>
-      </c>
-      <c r="C141" t="s">
-        <v>282</v>
       </c>
       <c r="D141">
         <v>50</v>
@@ -4055,10 +4058,10 @@
         <v>348</v>
       </c>
       <c r="B142" t="s">
+        <v>282</v>
+      </c>
+      <c r="C142" t="s">
         <v>283</v>
-      </c>
-      <c r="C142" t="s">
-        <v>284</v>
       </c>
       <c r="D142">
         <v>50</v>
@@ -4069,10 +4072,10 @@
         <v>290</v>
       </c>
       <c r="B143" t="s">
+        <v>284</v>
+      </c>
+      <c r="C143" t="s">
         <v>285</v>
-      </c>
-      <c r="C143" t="s">
-        <v>286</v>
       </c>
       <c r="D143">
         <v>80</v>
@@ -4083,10 +4086,10 @@
         <v>259</v>
       </c>
       <c r="B144" t="s">
+        <v>286</v>
+      </c>
+      <c r="C144" t="s">
         <v>287</v>
-      </c>
-      <c r="C144" t="s">
-        <v>288</v>
       </c>
       <c r="D144">
         <v>60</v>
@@ -4097,10 +4100,10 @@
         <v>261</v>
       </c>
       <c r="B145" t="s">
+        <v>288</v>
+      </c>
+      <c r="C145" t="s">
         <v>289</v>
-      </c>
-      <c r="C145" t="s">
-        <v>290</v>
       </c>
       <c r="D145">
         <v>60</v>
@@ -4111,10 +4114,10 @@
         <v>319</v>
       </c>
       <c r="B146" t="s">
+        <v>290</v>
+      </c>
+      <c r="C146" t="s">
         <v>291</v>
-      </c>
-      <c r="C146" t="s">
-        <v>292</v>
       </c>
       <c r="D146">
         <v>49.9</v>
@@ -4125,10 +4128,10 @@
         <v>325</v>
       </c>
       <c r="B147" t="s">
+        <v>292</v>
+      </c>
+      <c r="C147" t="s">
         <v>293</v>
-      </c>
-      <c r="C147" t="s">
-        <v>294</v>
       </c>
       <c r="D147">
         <v>49.9</v>
@@ -4139,10 +4142,10 @@
         <v>277</v>
       </c>
       <c r="B148" t="s">
+        <v>294</v>
+      </c>
+      <c r="C148" t="s">
         <v>295</v>
-      </c>
-      <c r="C148" t="s">
-        <v>296</v>
       </c>
       <c r="D148">
         <v>32.270000000000003</v>
@@ -4153,10 +4156,10 @@
         <v>281</v>
       </c>
       <c r="B149" t="s">
+        <v>296</v>
+      </c>
+      <c r="C149" t="s">
         <v>297</v>
-      </c>
-      <c r="C149" t="s">
-        <v>298</v>
       </c>
       <c r="D149">
         <v>32.270000000000003</v>
@@ -4167,10 +4170,10 @@
         <v>249</v>
       </c>
       <c r="B150" t="s">
+        <v>298</v>
+      </c>
+      <c r="C150" t="s">
         <v>299</v>
-      </c>
-      <c r="C150" t="s">
-        <v>300</v>
       </c>
       <c r="D150">
         <v>31.47</v>
@@ -4181,10 +4184,10 @@
         <v>263</v>
       </c>
       <c r="B151" t="s">
+        <v>300</v>
+      </c>
+      <c r="C151" t="s">
         <v>301</v>
-      </c>
-      <c r="C151" t="s">
-        <v>302</v>
       </c>
       <c r="D151">
         <v>32.49</v>
@@ -4195,10 +4198,10 @@
         <v>253</v>
       </c>
       <c r="B152" t="s">
+        <v>302</v>
+      </c>
+      <c r="C152" t="s">
         <v>303</v>
-      </c>
-      <c r="C152" t="s">
-        <v>304</v>
       </c>
       <c r="D152">
         <v>31.94</v>
@@ -4209,10 +4212,10 @@
         <v>287</v>
       </c>
       <c r="B153" t="s">
+        <v>304</v>
+      </c>
+      <c r="C153" t="s">
         <v>305</v>
-      </c>
-      <c r="C153" t="s">
-        <v>306</v>
       </c>
       <c r="D153">
         <v>35.79</v>
@@ -4223,10 +4226,10 @@
         <v>298</v>
       </c>
       <c r="B154" t="s">
+        <v>306</v>
+      </c>
+      <c r="C154" t="s">
         <v>307</v>
-      </c>
-      <c r="C154" t="s">
-        <v>308</v>
       </c>
       <c r="D154">
         <v>37.99</v>
@@ -4237,10 +4240,10 @@
         <v>270</v>
       </c>
       <c r="B155" t="s">
+        <v>308</v>
+      </c>
+      <c r="C155" t="s">
         <v>309</v>
-      </c>
-      <c r="C155" t="s">
-        <v>310</v>
       </c>
       <c r="D155">
         <v>32.49</v>
@@ -4251,10 +4254,10 @@
         <v>329</v>
       </c>
       <c r="B156" t="s">
+        <v>310</v>
+      </c>
+      <c r="C156" t="s">
         <v>311</v>
-      </c>
-      <c r="C156" t="s">
-        <v>312</v>
       </c>
       <c r="D156">
         <v>50</v>
@@ -4265,10 +4268,10 @@
         <v>330</v>
       </c>
       <c r="B157" t="s">
+        <v>312</v>
+      </c>
+      <c r="C157" t="s">
         <v>313</v>
-      </c>
-      <c r="C157" t="s">
-        <v>314</v>
       </c>
       <c r="D157">
         <v>63.5</v>
@@ -4279,10 +4282,10 @@
         <v>293</v>
       </c>
       <c r="B158" t="s">
+        <v>314</v>
+      </c>
+      <c r="C158" t="s">
         <v>315</v>
-      </c>
-      <c r="C158" t="s">
-        <v>316</v>
       </c>
       <c r="D158">
         <v>39.9</v>
@@ -4293,10 +4296,10 @@
         <v>313</v>
       </c>
       <c r="B159" t="s">
+        <v>316</v>
+      </c>
+      <c r="C159" t="s">
         <v>317</v>
-      </c>
-      <c r="C159" t="s">
-        <v>318</v>
       </c>
       <c r="D159">
         <v>40</v>
@@ -4307,10 +4310,10 @@
         <v>357</v>
       </c>
       <c r="B160" t="s">
+        <v>318</v>
+      </c>
+      <c r="C160" t="s">
         <v>319</v>
-      </c>
-      <c r="C160" t="s">
-        <v>320</v>
       </c>
       <c r="D160">
         <v>65</v>
@@ -4321,10 +4324,10 @@
         <v>358</v>
       </c>
       <c r="B161" t="s">
+        <v>320</v>
+      </c>
+      <c r="C161" t="s">
         <v>321</v>
-      </c>
-      <c r="C161" t="s">
-        <v>322</v>
       </c>
       <c r="D161">
         <v>70</v>
@@ -4335,10 +4338,10 @@
         <v>354</v>
       </c>
       <c r="B162" t="s">
+        <v>322</v>
+      </c>
+      <c r="C162" t="s">
         <v>323</v>
-      </c>
-      <c r="C162" t="s">
-        <v>324</v>
       </c>
       <c r="D162">
         <v>60</v>
@@ -4349,10 +4352,10 @@
         <v>668</v>
       </c>
       <c r="B163" t="s">
+        <v>324</v>
+      </c>
+      <c r="C163" t="s">
         <v>325</v>
-      </c>
-      <c r="C163" t="s">
-        <v>326</v>
       </c>
       <c r="D163">
         <v>149.99</v>
@@ -4363,10 +4366,10 @@
         <v>669</v>
       </c>
       <c r="B164" t="s">
+        <v>326</v>
+      </c>
+      <c r="C164" t="s">
         <v>327</v>
-      </c>
-      <c r="C164" t="s">
-        <v>328</v>
       </c>
       <c r="D164">
         <v>149.99</v>
@@ -4377,10 +4380,10 @@
         <v>772</v>
       </c>
       <c r="B165" t="s">
+        <v>328</v>
+      </c>
+      <c r="C165" t="s">
         <v>329</v>
-      </c>
-      <c r="C165" t="s">
-        <v>330</v>
       </c>
       <c r="D165">
         <v>45.44</v>
@@ -4391,10 +4394,10 @@
         <v>1356</v>
       </c>
       <c r="B166" t="s">
+        <v>330</v>
+      </c>
+      <c r="C166" t="s">
         <v>331</v>
-      </c>
-      <c r="C166" t="s">
-        <v>332</v>
       </c>
       <c r="D166">
         <v>16.600000000000001</v>
@@ -4405,10 +4408,10 @@
         <v>751</v>
       </c>
       <c r="B167" t="s">
+        <v>332</v>
+      </c>
+      <c r="C167" t="s">
         <v>333</v>
-      </c>
-      <c r="C167" t="s">
-        <v>334</v>
       </c>
       <c r="D167">
         <v>27.7</v>
@@ -4419,10 +4422,10 @@
         <v>1410</v>
       </c>
       <c r="B168" t="s">
+        <v>334</v>
+      </c>
+      <c r="C168" t="s">
         <v>335</v>
-      </c>
-      <c r="C168" t="s">
-        <v>336</v>
       </c>
       <c r="D168">
         <v>25</v>
@@ -4433,10 +4436,10 @@
         <v>677</v>
       </c>
       <c r="B169" t="s">
+        <v>336</v>
+      </c>
+      <c r="C169" t="s">
         <v>337</v>
-      </c>
-      <c r="C169" t="s">
-        <v>338</v>
       </c>
       <c r="D169">
         <v>38</v>
@@ -4447,10 +4450,10 @@
         <v>673</v>
       </c>
       <c r="B170" t="s">
+        <v>338</v>
+      </c>
+      <c r="C170" t="s">
         <v>339</v>
-      </c>
-      <c r="C170" t="s">
-        <v>340</v>
       </c>
       <c r="D170">
         <v>38</v>
@@ -4461,10 +4464,10 @@
         <v>740</v>
       </c>
       <c r="B171" t="s">
+        <v>340</v>
+      </c>
+      <c r="C171" t="s">
         <v>341</v>
-      </c>
-      <c r="C171" t="s">
-        <v>342</v>
       </c>
       <c r="D171">
         <v>20</v>
@@ -4475,10 +4478,10 @@
         <v>741</v>
       </c>
       <c r="B172" t="s">
+        <v>342</v>
+      </c>
+      <c r="C172" t="s">
         <v>343</v>
-      </c>
-      <c r="C172" t="s">
-        <v>344</v>
       </c>
       <c r="D172">
         <v>20</v>
@@ -4489,10 +4492,10 @@
         <v>739</v>
       </c>
       <c r="B173" t="s">
+        <v>344</v>
+      </c>
+      <c r="C173" t="s">
         <v>345</v>
-      </c>
-      <c r="C173" t="s">
-        <v>346</v>
       </c>
       <c r="D173">
         <v>20</v>
@@ -4503,10 +4506,10 @@
         <v>409</v>
       </c>
       <c r="B174" t="s">
+        <v>346</v>
+      </c>
+      <c r="C174" t="s">
         <v>347</v>
-      </c>
-      <c r="C174" t="s">
-        <v>348</v>
       </c>
       <c r="D174">
         <v>44.51</v>
@@ -4517,10 +4520,10 @@
         <v>419</v>
       </c>
       <c r="B175" t="s">
+        <v>348</v>
+      </c>
+      <c r="C175" t="s">
         <v>349</v>
-      </c>
-      <c r="C175" t="s">
-        <v>350</v>
       </c>
       <c r="D175">
         <v>6.9</v>
@@ -4531,10 +4534,10 @@
         <v>369</v>
       </c>
       <c r="B176" t="s">
+        <v>350</v>
+      </c>
+      <c r="C176" t="s">
         <v>351</v>
-      </c>
-      <c r="C176" t="s">
-        <v>352</v>
       </c>
       <c r="D176">
         <v>13</v>
@@ -4545,10 +4548,10 @@
         <v>375</v>
       </c>
       <c r="B177" t="s">
+        <v>352</v>
+      </c>
+      <c r="C177" t="s">
         <v>353</v>
-      </c>
-      <c r="C177" t="s">
-        <v>354</v>
       </c>
       <c r="D177">
         <v>20</v>
@@ -4559,10 +4562,10 @@
         <v>414</v>
       </c>
       <c r="B178" t="s">
+        <v>354</v>
+      </c>
+      <c r="C178" t="s">
         <v>355</v>
-      </c>
-      <c r="C178" t="s">
-        <v>356</v>
       </c>
       <c r="D178">
         <v>5.45</v>
@@ -4573,10 +4576,10 @@
         <v>1353</v>
       </c>
       <c r="B179" t="s">
+        <v>356</v>
+      </c>
+      <c r="C179" t="s">
         <v>357</v>
-      </c>
-      <c r="C179" t="s">
-        <v>358</v>
       </c>
       <c r="D179">
         <v>40</v>
@@ -4587,10 +4590,10 @@
         <v>388</v>
       </c>
       <c r="B180" t="s">
+        <v>358</v>
+      </c>
+      <c r="C180" t="s">
         <v>359</v>
-      </c>
-      <c r="C180" t="s">
-        <v>360</v>
       </c>
       <c r="D180">
         <v>40</v>
@@ -4601,10 +4604,10 @@
         <v>700</v>
       </c>
       <c r="B181" t="s">
+        <v>360</v>
+      </c>
+      <c r="C181" t="s">
         <v>361</v>
-      </c>
-      <c r="C181" t="s">
-        <v>362</v>
       </c>
       <c r="D181">
         <v>75</v>
@@ -4615,10 +4618,10 @@
         <v>702</v>
       </c>
       <c r="B182" t="s">
+        <v>362</v>
+      </c>
+      <c r="C182" t="s">
         <v>363</v>
-      </c>
-      <c r="C182" t="s">
-        <v>364</v>
       </c>
       <c r="D182">
         <v>75</v>
@@ -4629,10 +4632,10 @@
         <v>699</v>
       </c>
       <c r="B183" t="s">
+        <v>364</v>
+      </c>
+      <c r="C183" t="s">
         <v>365</v>
-      </c>
-      <c r="C183" t="s">
-        <v>366</v>
       </c>
       <c r="D183">
         <v>75</v>
@@ -4643,10 +4646,10 @@
         <v>392</v>
       </c>
       <c r="B184" t="s">
+        <v>366</v>
+      </c>
+      <c r="C184" t="s">
         <v>367</v>
-      </c>
-      <c r="C184" t="s">
-        <v>368</v>
       </c>
       <c r="D184">
         <v>55.84</v>
@@ -4657,10 +4660,10 @@
         <v>393</v>
       </c>
       <c r="B185" t="s">
+        <v>368</v>
+      </c>
+      <c r="C185" t="s">
         <v>369</v>
-      </c>
-      <c r="C185" t="s">
-        <v>370</v>
       </c>
       <c r="D185">
         <v>55.84</v>
@@ -4671,10 +4674,10 @@
         <v>394</v>
       </c>
       <c r="B186" t="s">
+        <v>370</v>
+      </c>
+      <c r="C186" t="s">
         <v>371</v>
-      </c>
-      <c r="C186" t="s">
-        <v>372</v>
       </c>
       <c r="D186">
         <v>55.84</v>
@@ -4685,10 +4688,10 @@
         <v>397</v>
       </c>
       <c r="B187" t="s">
+        <v>372</v>
+      </c>
+      <c r="C187" t="s">
         <v>373</v>
-      </c>
-      <c r="C187" t="s">
-        <v>374</v>
       </c>
       <c r="D187">
         <v>50.89</v>
@@ -4699,10 +4702,10 @@
         <v>1361</v>
       </c>
       <c r="B188" t="s">
+        <v>374</v>
+      </c>
+      <c r="C188" t="s">
         <v>375</v>
-      </c>
-      <c r="C188" t="s">
-        <v>376</v>
       </c>
       <c r="D188">
         <v>50</v>
@@ -4713,10 +4716,10 @@
         <v>378</v>
       </c>
       <c r="B189" t="s">
+        <v>376</v>
+      </c>
+      <c r="C189" t="s">
         <v>377</v>
-      </c>
-      <c r="C189" t="s">
-        <v>378</v>
       </c>
       <c r="D189">
         <v>20</v>
@@ -4727,10 +4730,10 @@
         <v>402</v>
       </c>
       <c r="B190" t="s">
+        <v>378</v>
+      </c>
+      <c r="C190" t="s">
         <v>379</v>
-      </c>
-      <c r="C190" t="s">
-        <v>380</v>
       </c>
       <c r="D190">
         <v>30</v>
@@ -4744,7 +4747,7 @@
         <v>2093</v>
       </c>
       <c r="C191" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D191">
         <v>30</v>
@@ -4755,10 +4758,10 @@
         <v>403</v>
       </c>
       <c r="B192" t="s">
+        <v>381</v>
+      </c>
+      <c r="C192" t="s">
         <v>382</v>
-      </c>
-      <c r="C192" t="s">
-        <v>383</v>
       </c>
       <c r="D192">
         <v>30</v>
@@ -4769,10 +4772,10 @@
         <v>725</v>
       </c>
       <c r="B193" t="s">
+        <v>383</v>
+      </c>
+      <c r="C193" t="s">
         <v>384</v>
-      </c>
-      <c r="C193" t="s">
-        <v>385</v>
       </c>
       <c r="D193">
         <v>70</v>
@@ -4783,10 +4786,10 @@
         <v>724</v>
       </c>
       <c r="B194" t="s">
+        <v>385</v>
+      </c>
+      <c r="C194" t="s">
         <v>386</v>
-      </c>
-      <c r="C194" t="s">
-        <v>387</v>
       </c>
       <c r="D194">
         <v>50</v>
@@ -4797,10 +4800,10 @@
         <v>832</v>
       </c>
       <c r="B195" t="s">
+        <v>387</v>
+      </c>
+      <c r="C195" t="s">
         <v>388</v>
-      </c>
-      <c r="C195" t="s">
-        <v>389</v>
       </c>
       <c r="D195">
         <v>50</v>
@@ -4811,10 +4814,10 @@
         <v>705</v>
       </c>
       <c r="B196" t="s">
+        <v>389</v>
+      </c>
+      <c r="C196" t="s">
         <v>390</v>
-      </c>
-      <c r="C196" t="s">
-        <v>391</v>
       </c>
       <c r="D196">
         <v>60</v>
@@ -4825,10 +4828,10 @@
         <v>707</v>
       </c>
       <c r="B197" t="s">
+        <v>391</v>
+      </c>
+      <c r="C197" t="s">
         <v>392</v>
-      </c>
-      <c r="C197" t="s">
-        <v>393</v>
       </c>
       <c r="D197">
         <v>60</v>
@@ -4839,10 +4842,10 @@
         <v>695</v>
       </c>
       <c r="B198" t="s">
+        <v>393</v>
+      </c>
+      <c r="C198" t="s">
         <v>394</v>
-      </c>
-      <c r="C198" t="s">
-        <v>395</v>
       </c>
       <c r="D198">
         <v>60</v>
@@ -4853,10 +4856,10 @@
         <v>713</v>
       </c>
       <c r="B199" t="s">
+        <v>395</v>
+      </c>
+      <c r="C199" t="s">
         <v>396</v>
-      </c>
-      <c r="C199" t="s">
-        <v>397</v>
       </c>
       <c r="D199">
         <v>60</v>
@@ -4867,10 +4870,10 @@
         <v>714</v>
       </c>
       <c r="B200" t="s">
+        <v>397</v>
+      </c>
+      <c r="C200" t="s">
         <v>398</v>
-      </c>
-      <c r="C200" t="s">
-        <v>399</v>
       </c>
       <c r="D200">
         <v>60</v>
@@ -4881,10 +4884,10 @@
         <v>719</v>
       </c>
       <c r="B201" t="s">
+        <v>399</v>
+      </c>
+      <c r="C201" t="s">
         <v>400</v>
-      </c>
-      <c r="C201" t="s">
-        <v>401</v>
       </c>
       <c r="D201">
         <v>60</v>
@@ -4895,10 +4898,10 @@
         <v>720</v>
       </c>
       <c r="B202" t="s">
+        <v>401</v>
+      </c>
+      <c r="C202" t="s">
         <v>402</v>
-      </c>
-      <c r="C202" t="s">
-        <v>403</v>
       </c>
       <c r="D202">
         <v>60</v>
@@ -4909,10 +4912,10 @@
         <v>723</v>
       </c>
       <c r="B203" t="s">
+        <v>403</v>
+      </c>
+      <c r="C203" t="s">
         <v>404</v>
-      </c>
-      <c r="C203" t="s">
-        <v>405</v>
       </c>
       <c r="D203">
         <v>60</v>
@@ -4923,10 +4926,10 @@
         <v>712</v>
       </c>
       <c r="B204" t="s">
+        <v>405</v>
+      </c>
+      <c r="C204" t="s">
         <v>406</v>
-      </c>
-      <c r="C204" t="s">
-        <v>407</v>
       </c>
       <c r="D204">
         <v>60</v>
@@ -4937,10 +4940,10 @@
         <v>721</v>
       </c>
       <c r="B205" t="s">
+        <v>407</v>
+      </c>
+      <c r="C205" t="s">
         <v>408</v>
-      </c>
-      <c r="C205" t="s">
-        <v>409</v>
       </c>
       <c r="D205">
         <v>60</v>
@@ -4951,10 +4954,10 @@
         <v>718</v>
       </c>
       <c r="B206" t="s">
+        <v>409</v>
+      </c>
+      <c r="C206" t="s">
         <v>410</v>
-      </c>
-      <c r="C206" t="s">
-        <v>411</v>
       </c>
       <c r="D206">
         <v>60</v>
@@ -4965,10 +4968,10 @@
         <v>381</v>
       </c>
       <c r="B207" t="s">
+        <v>411</v>
+      </c>
+      <c r="C207" t="s">
         <v>412</v>
-      </c>
-      <c r="C207" t="s">
-        <v>413</v>
       </c>
       <c r="D207">
         <v>60</v>
@@ -4979,10 +4982,10 @@
         <v>788</v>
       </c>
       <c r="B208" t="s">
+        <v>413</v>
+      </c>
+      <c r="C208" t="s">
         <v>414</v>
-      </c>
-      <c r="C208" t="s">
-        <v>415</v>
       </c>
       <c r="D208">
         <v>30</v>
@@ -4993,10 +4996,10 @@
         <v>384</v>
       </c>
       <c r="B209" t="s">
+        <v>415</v>
+      </c>
+      <c r="C209" t="s">
         <v>416</v>
-      </c>
-      <c r="C209" t="s">
-        <v>417</v>
       </c>
       <c r="D209">
         <v>50</v>
@@ -5007,10 +5010,10 @@
         <v>385</v>
       </c>
       <c r="B210" t="s">
+        <v>417</v>
+      </c>
+      <c r="C210" t="s">
         <v>418</v>
-      </c>
-      <c r="C210" t="s">
-        <v>419</v>
       </c>
       <c r="D210">
         <v>50</v>
@@ -5021,10 +5024,10 @@
         <v>386</v>
       </c>
       <c r="B211" t="s">
+        <v>419</v>
+      </c>
+      <c r="C211" t="s">
         <v>420</v>
-      </c>
-      <c r="C211" t="s">
-        <v>421</v>
       </c>
       <c r="D211">
         <v>50</v>
@@ -5035,10 +5038,10 @@
         <v>387</v>
       </c>
       <c r="B212" t="s">
+        <v>421</v>
+      </c>
+      <c r="C212" t="s">
         <v>422</v>
-      </c>
-      <c r="C212" t="s">
-        <v>423</v>
       </c>
       <c r="D212">
         <v>50</v>
@@ -5049,10 +5052,10 @@
         <v>389</v>
       </c>
       <c r="B213" t="s">
+        <v>423</v>
+      </c>
+      <c r="C213" t="s">
         <v>424</v>
-      </c>
-      <c r="C213" t="s">
-        <v>425</v>
       </c>
       <c r="D213">
         <v>50</v>
@@ -5063,10 +5066,10 @@
         <v>390</v>
       </c>
       <c r="B214" t="s">
+        <v>425</v>
+      </c>
+      <c r="C214" t="s">
         <v>426</v>
-      </c>
-      <c r="C214" t="s">
-        <v>427</v>
       </c>
       <c r="D214">
         <v>50</v>
@@ -5077,10 +5080,10 @@
         <v>391</v>
       </c>
       <c r="B215" t="s">
+        <v>427</v>
+      </c>
+      <c r="C215" t="s">
         <v>428</v>
-      </c>
-      <c r="C215" t="s">
-        <v>429</v>
       </c>
       <c r="D215">
         <v>50</v>
@@ -5091,10 +5094,10 @@
         <v>1216</v>
       </c>
       <c r="B216" t="s">
+        <v>429</v>
+      </c>
+      <c r="C216" t="s">
         <v>430</v>
-      </c>
-      <c r="C216" t="s">
-        <v>431</v>
       </c>
       <c r="D216">
         <v>50</v>
@@ -5105,10 +5108,10 @@
         <v>1215</v>
       </c>
       <c r="B217" t="s">
+        <v>431</v>
+      </c>
+      <c r="C217" t="s">
         <v>432</v>
-      </c>
-      <c r="C217" t="s">
-        <v>433</v>
       </c>
       <c r="D217">
         <v>42.22</v>
@@ -5119,10 +5122,10 @@
         <v>424</v>
       </c>
       <c r="B218" t="s">
+        <v>433</v>
+      </c>
+      <c r="C218" t="s">
         <v>434</v>
-      </c>
-      <c r="C218" t="s">
-        <v>435</v>
       </c>
       <c r="D218">
         <v>30</v>
@@ -5136,7 +5139,7 @@
         <v>18503</v>
       </c>
       <c r="C219" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D219">
         <v>30</v>
@@ -5147,10 +5150,10 @@
         <v>691</v>
       </c>
       <c r="B220" t="s">
+        <v>436</v>
+      </c>
+      <c r="C220" t="s">
         <v>437</v>
-      </c>
-      <c r="C220" t="s">
-        <v>438</v>
       </c>
       <c r="D220">
         <v>94.44</v>
@@ -5161,10 +5164,10 @@
         <v>455</v>
       </c>
       <c r="B221" t="s">
+        <v>438</v>
+      </c>
+      <c r="C221" t="s">
         <v>439</v>
-      </c>
-      <c r="C221" t="s">
-        <v>440</v>
       </c>
       <c r="D221">
         <v>25</v>
@@ -5175,10 +5178,10 @@
         <v>459</v>
       </c>
       <c r="B222" t="s">
+        <v>440</v>
+      </c>
+      <c r="C222" t="s">
         <v>441</v>
-      </c>
-      <c r="C222" t="s">
-        <v>442</v>
       </c>
       <c r="D222">
         <v>25</v>
@@ -5189,10 +5192,10 @@
         <v>461</v>
       </c>
       <c r="B223" t="s">
+        <v>442</v>
+      </c>
+      <c r="C223" t="s">
         <v>443</v>
-      </c>
-      <c r="C223" t="s">
-        <v>444</v>
       </c>
       <c r="D223">
         <v>25</v>
@@ -5203,10 +5206,10 @@
         <v>463</v>
       </c>
       <c r="B224" t="s">
+        <v>444</v>
+      </c>
+      <c r="C224" t="s">
         <v>445</v>
-      </c>
-      <c r="C224" t="s">
-        <v>446</v>
       </c>
       <c r="D224">
         <v>29.9</v>
@@ -5217,10 +5220,10 @@
         <v>464</v>
       </c>
       <c r="B225" t="s">
+        <v>446</v>
+      </c>
+      <c r="C225" t="s">
         <v>447</v>
-      </c>
-      <c r="C225" t="s">
-        <v>448</v>
       </c>
       <c r="D225">
         <v>29.9</v>
@@ -5231,10 +5234,10 @@
         <v>689</v>
       </c>
       <c r="B226" t="s">
+        <v>448</v>
+      </c>
+      <c r="C226" t="s">
         <v>449</v>
-      </c>
-      <c r="C226" t="s">
-        <v>450</v>
       </c>
       <c r="D226">
         <v>30</v>
@@ -5245,10 +5248,10 @@
         <v>429</v>
       </c>
       <c r="B227" t="s">
+        <v>450</v>
+      </c>
+      <c r="C227" t="s">
         <v>451</v>
-      </c>
-      <c r="C227" t="s">
-        <v>452</v>
       </c>
       <c r="D227">
         <v>30</v>
@@ -5259,10 +5262,10 @@
         <v>784</v>
       </c>
       <c r="B228" t="s">
+        <v>452</v>
+      </c>
+      <c r="C228" t="s">
         <v>453</v>
-      </c>
-      <c r="C228" t="s">
-        <v>454</v>
       </c>
       <c r="D228">
         <v>9.4499999999999993</v>
@@ -5273,10 +5276,10 @@
         <v>786</v>
       </c>
       <c r="B229" t="s">
+        <v>454</v>
+      </c>
+      <c r="C229" t="s">
         <v>455</v>
-      </c>
-      <c r="C229" t="s">
-        <v>456</v>
       </c>
       <c r="D229">
         <v>9.4499999999999993</v>
@@ -5287,10 +5290,10 @@
         <v>434</v>
       </c>
       <c r="B230" t="s">
+        <v>456</v>
+      </c>
+      <c r="C230" t="s">
         <v>457</v>
-      </c>
-      <c r="C230" t="s">
-        <v>458</v>
       </c>
       <c r="D230">
         <v>10</v>
@@ -5301,10 +5304,10 @@
         <v>448</v>
       </c>
       <c r="B231" t="s">
+        <v>458</v>
+      </c>
+      <c r="C231" t="s">
         <v>459</v>
-      </c>
-      <c r="C231" t="s">
-        <v>460</v>
       </c>
       <c r="D231">
         <v>10</v>
@@ -5315,10 +5318,10 @@
         <v>431</v>
       </c>
       <c r="B232" t="s">
+        <v>460</v>
+      </c>
+      <c r="C232" t="s">
         <v>461</v>
-      </c>
-      <c r="C232" t="s">
-        <v>462</v>
       </c>
       <c r="D232">
         <v>10</v>
@@ -5329,10 +5332,10 @@
         <v>1140</v>
       </c>
       <c r="B233" t="s">
+        <v>462</v>
+      </c>
+      <c r="C233" t="s">
         <v>463</v>
-      </c>
-      <c r="C233" t="s">
-        <v>464</v>
       </c>
       <c r="D233">
         <v>23.9</v>
@@ -5343,10 +5346,10 @@
         <v>517</v>
       </c>
       <c r="B234" t="s">
+        <v>464</v>
+      </c>
+      <c r="C234" t="s">
         <v>465</v>
-      </c>
-      <c r="C234" t="s">
-        <v>466</v>
       </c>
       <c r="D234">
         <v>23.9</v>
@@ -5357,10 +5360,10 @@
         <v>623</v>
       </c>
       <c r="B235" t="s">
+        <v>466</v>
+      </c>
+      <c r="C235" t="s">
         <v>467</v>
-      </c>
-      <c r="C235" t="s">
-        <v>468</v>
       </c>
       <c r="D235">
         <v>29.8</v>
@@ -5371,10 +5374,10 @@
         <v>1153</v>
       </c>
       <c r="B236" t="s">
+        <v>468</v>
+      </c>
+      <c r="C236" t="s">
         <v>469</v>
-      </c>
-      <c r="C236" t="s">
-        <v>470</v>
       </c>
       <c r="D236">
         <v>29.8</v>
@@ -5385,10 +5388,10 @@
         <v>520</v>
       </c>
       <c r="B237" t="s">
+        <v>470</v>
+      </c>
+      <c r="C237" t="s">
         <v>471</v>
-      </c>
-      <c r="C237" t="s">
-        <v>472</v>
       </c>
       <c r="D237">
         <v>29.8</v>
@@ -5399,10 +5402,10 @@
         <v>474</v>
       </c>
       <c r="B238" t="s">
+        <v>472</v>
+      </c>
+      <c r="C238" t="s">
         <v>473</v>
-      </c>
-      <c r="C238" t="s">
-        <v>474</v>
       </c>
       <c r="D238">
         <v>46.6</v>
@@ -5413,10 +5416,10 @@
         <v>467</v>
       </c>
       <c r="B239" t="s">
+        <v>474</v>
+      </c>
+      <c r="C239" t="s">
         <v>475</v>
-      </c>
-      <c r="C239" t="s">
-        <v>476</v>
       </c>
       <c r="D239">
         <v>30</v>
@@ -5427,10 +5430,10 @@
         <v>479</v>
       </c>
       <c r="B240" t="s">
+        <v>476</v>
+      </c>
+      <c r="C240" t="s">
         <v>477</v>
-      </c>
-      <c r="C240" t="s">
-        <v>478</v>
       </c>
       <c r="D240">
         <v>62.27</v>
@@ -5441,10 +5444,10 @@
         <v>501</v>
       </c>
       <c r="B241" t="s">
+        <v>478</v>
+      </c>
+      <c r="C241" t="s">
         <v>479</v>
-      </c>
-      <c r="C241" t="s">
-        <v>480</v>
       </c>
       <c r="D241">
         <v>30</v>
@@ -5455,10 +5458,10 @@
         <v>764</v>
       </c>
       <c r="B242" t="s">
+        <v>480</v>
+      </c>
+      <c r="C242" t="s">
         <v>481</v>
-      </c>
-      <c r="C242" t="s">
-        <v>482</v>
       </c>
       <c r="D242">
         <v>35.04</v>
@@ -5469,10 +5472,10 @@
         <v>768</v>
       </c>
       <c r="B243" t="s">
+        <v>482</v>
+      </c>
+      <c r="C243" t="s">
         <v>483</v>
-      </c>
-      <c r="C243" t="s">
-        <v>484</v>
       </c>
       <c r="D243">
         <v>70.14</v>
@@ -5483,10 +5486,10 @@
         <v>761</v>
       </c>
       <c r="B244" t="s">
+        <v>484</v>
+      </c>
+      <c r="C244" t="s">
         <v>485</v>
-      </c>
-      <c r="C244" t="s">
-        <v>486</v>
       </c>
       <c r="D244">
         <v>35</v>
@@ -5497,10 +5500,10 @@
         <v>765</v>
       </c>
       <c r="B245" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C245" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D245">
         <v>70</v>
@@ -5511,10 +5514,10 @@
         <v>487</v>
       </c>
       <c r="B246" t="s">
+        <v>487</v>
+      </c>
+      <c r="C246" t="s">
         <v>488</v>
-      </c>
-      <c r="C246" t="s">
-        <v>489</v>
       </c>
       <c r="D246">
         <v>30</v>
@@ -5525,10 +5528,10 @@
         <v>488</v>
       </c>
       <c r="B247" t="s">
+        <v>489</v>
+      </c>
+      <c r="C247" t="s">
         <v>490</v>
-      </c>
-      <c r="C247" t="s">
-        <v>491</v>
       </c>
       <c r="D247">
         <v>30</v>
@@ -5539,10 +5542,10 @@
         <v>490</v>
       </c>
       <c r="B248" t="s">
+        <v>491</v>
+      </c>
+      <c r="C248" t="s">
         <v>492</v>
-      </c>
-      <c r="C248" t="s">
-        <v>493</v>
       </c>
       <c r="D248">
         <v>30</v>
@@ -5553,10 +5556,10 @@
         <v>512</v>
       </c>
       <c r="B249" t="s">
+        <v>493</v>
+      </c>
+      <c r="C249" t="s">
         <v>494</v>
-      </c>
-      <c r="C249" t="s">
-        <v>495</v>
       </c>
       <c r="D249">
         <v>30</v>
@@ -5567,10 +5570,10 @@
         <v>494</v>
       </c>
       <c r="B250" t="s">
+        <v>495</v>
+      </c>
+      <c r="C250" t="s">
         <v>496</v>
-      </c>
-      <c r="C250" t="s">
-        <v>497</v>
       </c>
       <c r="D250">
         <v>30</v>
@@ -5581,10 +5584,10 @@
         <v>495</v>
       </c>
       <c r="B251" t="s">
+        <v>497</v>
+      </c>
+      <c r="C251" t="s">
         <v>498</v>
-      </c>
-      <c r="C251" t="s">
-        <v>499</v>
       </c>
       <c r="D251">
         <v>30</v>
@@ -5595,10 +5598,10 @@
         <v>504</v>
       </c>
       <c r="B252" t="s">
+        <v>499</v>
+      </c>
+      <c r="C252" t="s">
         <v>500</v>
-      </c>
-      <c r="C252" t="s">
-        <v>501</v>
       </c>
       <c r="D252">
         <v>30</v>
@@ -5609,10 +5612,10 @@
         <v>505</v>
       </c>
       <c r="B253" t="s">
+        <v>501</v>
+      </c>
+      <c r="C253" t="s">
         <v>502</v>
-      </c>
-      <c r="C253" t="s">
-        <v>503</v>
       </c>
       <c r="D253">
         <v>30</v>
@@ -5623,10 +5626,10 @@
         <v>506</v>
       </c>
       <c r="B254" t="s">
+        <v>503</v>
+      </c>
+      <c r="C254" t="s">
         <v>504</v>
-      </c>
-      <c r="C254" t="s">
-        <v>505</v>
       </c>
       <c r="D254">
         <v>30</v>
@@ -5637,10 +5640,10 @@
         <v>507</v>
       </c>
       <c r="B255" t="s">
+        <v>505</v>
+      </c>
+      <c r="C255" t="s">
         <v>506</v>
-      </c>
-      <c r="C255" t="s">
-        <v>507</v>
       </c>
       <c r="D255">
         <v>30</v>
@@ -5651,10 +5654,10 @@
         <v>508</v>
       </c>
       <c r="B256" t="s">
+        <v>507</v>
+      </c>
+      <c r="C256" t="s">
         <v>508</v>
-      </c>
-      <c r="C256" t="s">
-        <v>509</v>
       </c>
       <c r="D256">
         <v>30</v>
@@ -5665,10 +5668,10 @@
         <v>509</v>
       </c>
       <c r="B257" t="s">
+        <v>509</v>
+      </c>
+      <c r="C257" t="s">
         <v>510</v>
-      </c>
-      <c r="C257" t="s">
-        <v>511</v>
       </c>
       <c r="D257">
         <v>30</v>
@@ -5679,10 +5682,10 @@
         <v>510</v>
       </c>
       <c r="B258" t="s">
+        <v>511</v>
+      </c>
+      <c r="C258" t="s">
         <v>512</v>
-      </c>
-      <c r="C258" t="s">
-        <v>513</v>
       </c>
       <c r="D258">
         <v>30</v>
@@ -5693,10 +5696,10 @@
         <v>511</v>
       </c>
       <c r="B259" t="s">
+        <v>513</v>
+      </c>
+      <c r="C259" t="s">
         <v>514</v>
-      </c>
-      <c r="C259" t="s">
-        <v>515</v>
       </c>
       <c r="D259">
         <v>30</v>
@@ -5707,10 +5710,10 @@
         <v>685</v>
       </c>
       <c r="B260" t="s">
+        <v>515</v>
+      </c>
+      <c r="C260" t="s">
         <v>516</v>
-      </c>
-      <c r="C260" t="s">
-        <v>517</v>
       </c>
       <c r="D260">
         <v>54.29</v>
@@ -5721,10 +5724,10 @@
         <v>1496</v>
       </c>
       <c r="B261" t="s">
+        <v>517</v>
+      </c>
+      <c r="C261" t="s">
         <v>518</v>
-      </c>
-      <c r="C261" t="s">
-        <v>519</v>
       </c>
       <c r="D261">
         <v>7.79</v>
@@ -5735,10 +5738,10 @@
         <v>550</v>
       </c>
       <c r="B262" t="s">
+        <v>519</v>
+      </c>
+      <c r="C262" t="s">
         <v>520</v>
-      </c>
-      <c r="C262" t="s">
-        <v>521</v>
       </c>
       <c r="D262">
         <v>100</v>
@@ -5749,10 +5752,10 @@
         <v>551</v>
       </c>
       <c r="B263" t="s">
+        <v>521</v>
+      </c>
+      <c r="C263" t="s">
         <v>522</v>
-      </c>
-      <c r="C263" t="s">
-        <v>523</v>
       </c>
       <c r="D263">
         <v>100</v>
@@ -5763,10 +5766,10 @@
         <v>552</v>
       </c>
       <c r="B264" t="s">
+        <v>523</v>
+      </c>
+      <c r="C264" t="s">
         <v>524</v>
-      </c>
-      <c r="C264" t="s">
-        <v>525</v>
       </c>
       <c r="D264">
         <v>100</v>
@@ -5777,10 +5780,10 @@
         <v>553</v>
       </c>
       <c r="B265" t="s">
+        <v>525</v>
+      </c>
+      <c r="C265" t="s">
         <v>526</v>
-      </c>
-      <c r="C265" t="s">
-        <v>527</v>
       </c>
       <c r="D265">
         <v>100</v>
@@ -5791,10 +5794,10 @@
         <v>564</v>
       </c>
       <c r="B266" t="s">
+        <v>527</v>
+      </c>
+      <c r="C266" t="s">
         <v>528</v>
-      </c>
-      <c r="C266" t="s">
-        <v>529</v>
       </c>
       <c r="D266">
         <v>85.52</v>
@@ -5805,10 +5808,10 @@
         <v>525</v>
       </c>
       <c r="B267" t="s">
+        <v>529</v>
+      </c>
+      <c r="C267" t="s">
         <v>530</v>
-      </c>
-      <c r="C267" t="s">
-        <v>531</v>
       </c>
       <c r="D267">
         <v>25.62</v>
@@ -5819,10 +5822,10 @@
         <v>531</v>
       </c>
       <c r="B268" t="s">
+        <v>531</v>
+      </c>
+      <c r="C268" t="s">
         <v>532</v>
-      </c>
-      <c r="C268" t="s">
-        <v>533</v>
       </c>
       <c r="D268">
         <v>40</v>
@@ -5833,10 +5836,10 @@
         <v>533</v>
       </c>
       <c r="B269" t="s">
+        <v>533</v>
+      </c>
+      <c r="C269" t="s">
         <v>534</v>
-      </c>
-      <c r="C269" t="s">
-        <v>535</v>
       </c>
       <c r="D269">
         <v>40</v>
@@ -5847,10 +5850,10 @@
         <v>535</v>
       </c>
       <c r="B270" t="s">
+        <v>535</v>
+      </c>
+      <c r="C270" t="s">
         <v>536</v>
-      </c>
-      <c r="C270" t="s">
-        <v>537</v>
       </c>
       <c r="D270">
         <v>40</v>
@@ -5861,10 +5864,10 @@
         <v>1387</v>
       </c>
       <c r="B271" t="s">
+        <v>537</v>
+      </c>
+      <c r="C271" t="s">
         <v>538</v>
-      </c>
-      <c r="C271" t="s">
-        <v>539</v>
       </c>
       <c r="D271">
         <v>15</v>
@@ -5875,10 +5878,10 @@
         <v>573</v>
       </c>
       <c r="B272" t="s">
+        <v>539</v>
+      </c>
+      <c r="C272" t="s">
         <v>540</v>
-      </c>
-      <c r="C272" t="s">
-        <v>541</v>
       </c>
       <c r="D272">
         <v>75</v>
@@ -5889,10 +5892,10 @@
         <v>574</v>
       </c>
       <c r="B273" t="s">
+        <v>541</v>
+      </c>
+      <c r="C273" t="s">
         <v>542</v>
-      </c>
-      <c r="C273" t="s">
-        <v>543</v>
       </c>
       <c r="D273">
         <v>75</v>
@@ -5903,10 +5906,10 @@
         <v>577</v>
       </c>
       <c r="B274" t="s">
+        <v>543</v>
+      </c>
+      <c r="C274" t="s">
         <v>544</v>
-      </c>
-      <c r="C274" t="s">
-        <v>545</v>
       </c>
       <c r="D274">
         <v>75</v>
@@ -5917,10 +5920,10 @@
         <v>588</v>
       </c>
       <c r="B275" t="s">
+        <v>545</v>
+      </c>
+      <c r="C275" t="s">
         <v>546</v>
-      </c>
-      <c r="C275" t="s">
-        <v>547</v>
       </c>
       <c r="D275">
         <v>15</v>
@@ -5931,10 +5934,10 @@
         <v>594</v>
       </c>
       <c r="B276" t="s">
+        <v>547</v>
+      </c>
+      <c r="C276" t="s">
         <v>548</v>
-      </c>
-      <c r="C276" t="s">
-        <v>549</v>
       </c>
       <c r="D276">
         <v>83.88</v>
@@ -5945,10 +5948,10 @@
         <v>818</v>
       </c>
       <c r="B277" t="s">
+        <v>549</v>
+      </c>
+      <c r="C277" t="s">
         <v>550</v>
-      </c>
-      <c r="C277" t="s">
-        <v>551</v>
       </c>
       <c r="D277">
         <v>44.05</v>
@@ -5959,10 +5962,10 @@
         <v>813</v>
       </c>
       <c r="B278" t="s">
+        <v>551</v>
+      </c>
+      <c r="C278" t="s">
         <v>552</v>
-      </c>
-      <c r="C278" t="s">
-        <v>553</v>
       </c>
       <c r="D278">
         <v>48.11</v>
@@ -5973,10 +5976,10 @@
         <v>807</v>
       </c>
       <c r="B279" t="s">
+        <v>553</v>
+      </c>
+      <c r="C279" t="s">
         <v>554</v>
-      </c>
-      <c r="C279" t="s">
-        <v>555</v>
       </c>
       <c r="D279">
         <v>48.11</v>
@@ -5987,10 +5990,10 @@
         <v>823</v>
       </c>
       <c r="B280" t="s">
+        <v>555</v>
+      </c>
+      <c r="C280" t="s">
         <v>556</v>
-      </c>
-      <c r="C280" t="s">
-        <v>557</v>
       </c>
       <c r="D280">
         <v>44.4</v>
@@ -6001,10 +6004,10 @@
         <v>833</v>
       </c>
       <c r="B281" t="s">
+        <v>557</v>
+      </c>
+      <c r="C281" t="s">
         <v>558</v>
-      </c>
-      <c r="C281" t="s">
-        <v>559</v>
       </c>
       <c r="D281">
         <v>38.840000000000003</v>
@@ -6018,7 +6021,7 @@
         <v>7896042027890</v>
       </c>
       <c r="C282" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D282">
         <v>7.2</v>
@@ -6026,5 +6029,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>